<commit_message>
update evaluation with prompt data generated
</commit_message>
<xml_diff>
--- a/0_data/9_evaluation/comparison_model_evaluation.xlsx
+++ b/0_data/9_evaluation/comparison_model_evaluation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>d</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>d_prompts</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -489,6 +494,9 @@
       <c r="G2" t="n">
         <v>15.18</v>
       </c>
+      <c r="H2" t="n">
+        <v>15.1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -514,6 +522,9 @@
       <c r="G3" t="n">
         <v>11.72</v>
       </c>
+      <c r="H3" t="n">
+        <v>11.93</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -539,6 +550,9 @@
       <c r="G4" t="n">
         <v>3.38</v>
       </c>
+      <c r="H4" t="n">
+        <v>3.55</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -564,6 +578,9 @@
       <c r="G5" t="n">
         <v>19.82</v>
       </c>
+      <c r="H5" t="n">
+        <v>18.8</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -589,6 +606,9 @@
       <c r="G6" t="n">
         <v>5.95</v>
       </c>
+      <c r="H6" t="n">
+        <v>5.83</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -614,6 +634,9 @@
       <c r="G7" t="n">
         <v>0.02</v>
       </c>
+      <c r="H7" t="n">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -638,6 +661,9 @@
       </c>
       <c r="G8" t="n">
         <v>2.23</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2.1</v>
       </c>
     </row>
     <row r="9">
@@ -720,6 +746,13 @@
     0    0    0    0    0    0    0    0]</t>
         </is>
       </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[ 959  569 1357  483  177  200    4  175   27   20   16    0   18    0
+    3    1    0    0    0    0    0    0    0    0    0    0    0    0
+    0    0    0    0    0    0    0    0]</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -757,6 +790,11 @@
           <t>[5548   19 4520   24 5151  945   31 4855   20 5020   97 2094]</t>
         </is>
       </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>[831   1 576   0 696 313   1 620  19 576   1 390]</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -794,6 +832,11 @@
           <t>{'C': 5548, 'C#': 19, 'D': 4520, 'D#': 24, 'E': 5151, 'F': 945, 'F#': 31, 'G': 4855, 'G#': 20, 'A': 5020, 'A#': 97, 'B': 2094}</t>
         </is>
       </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>{'C': 831, 'C#': 1, 'D': 576, 'D#': 0, 'E': 696, 'F': 313, 'F#': 1, 'G': 620, 'G#': 19, 'A': 576, 'A#': 1, 'B': 390}</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -818,6 +861,9 @@
       </c>
       <c r="G12" t="n">
         <v>1.91</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.47</v>
       </c>
     </row>
     <row r="13">
@@ -922,6 +968,22 @@
  [ 692    0   84    0   64    8    0  194    2  639    2  397]]</t>
         </is>
       </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>[[211   0 203   0  59  19   0  48   1 104   0 183]
+ [  0   0   0   0   0   0   0   0   1   0   0   0]
+ [200   1 106   0 180  10   0  36   0  18   0  23]
+ [  0   0   0   0   0   0   0   0   0   0   0   0]
+ [ 71   0 200   0 144  81   0 110   2  71   0  13]
+ [ 12   0   7   0 109 116   0  58   1   7   0   2]
+ [  0   0   0   0   1   0   0   0   0   0   0   0]
+ [ 50   0  32   0 146  77   0 179   1 109   0  24]
+ [  2   0   0   0   0   0   0   1  11   3   1   1]
+ [ 91   0  18   0  51   8   1 153   2 158   0  92]
+ [  1   0   0   0   0   0   0   0   0   0   0   0]
+ [188   0  10   0   6   2   0  30   0 101   0  52]]</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -947,6 +1009,9 @@
       <c r="G14" t="n">
         <v>283.24</v>
       </c>
+      <c r="H14" t="n">
+        <v>268.27</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -972,6 +1037,9 @@
       <c r="G15" t="n">
         <v>6.17</v>
       </c>
+      <c r="H15" t="n">
+        <v>6.29</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -996,6 +1064,9 @@
       </c>
       <c r="G16" t="n">
         <v>2.87</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2.57</v>
       </c>
     </row>
     <row r="17">
@@ -1046,6 +1117,13 @@
     14     0     2     3    14     5     1     0]</t>
         </is>
       </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>[  79 1278 1302  621  380   68   56   32   85   16   14   10   20    8
+    9    6   22    7    3    0    2    0    1    0    0    0    0    0
+    1    0    0    0]</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1070,6 +1148,9 @@
       </c>
       <c r="G18" t="n">
         <v>6.07</v>
+      </c>
+      <c r="H18" t="n">
+        <v>6.25</v>
       </c>
     </row>
     <row r="19">
@@ -1138,6 +1219,15 @@
      0     0     0     0]</t>
         </is>
       </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>[   1 1186    0  918    0  243    0 1283    0   56    0   33   12   16
+    0  167    0    5   13    7    4    7    0   17    0    4    3    6
+    1    3    0   37    0    0    0    0    0    0    0    0    0    0
+    0    0    0    0    0    0    0    0    0    0    0    0    0    0
+    0    0    0    0    0    0    0    0]</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -1173,6 +1263,11 @@
       <c r="G20" t="inlineStr">
         <is>
           <t>{0: 0, 1: 17, 2: 10088, 3: 0, 4: 7136, 5: 0, 6: 1491, 7: 0, 8: 5857, 9: 0, 10: 646, 11: 0, 12: 445, 13: 160, 14: 194, 15: 0, 16: 1224, 17: 0, 18: 122, 19: 44, 20: 102, 21: 47, 22: 57, 23: 0, 24: 102, 25: 0, 26: 36, 27: 27, 28: 33, 29: 10, 30: 24, 31: 0, 32: 422}</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>{0: 0, 1: 1, 2: 1186, 3: 0, 4: 918, 5: 0, 6: 243, 7: 0, 8: 1283, 9: 0, 10: 56, 11: 0, 12: 33, 13: 12, 14: 16, 15: 0, 16: 167, 17: 0, 18: 5, 19: 13, 20: 7, 21: 4, 22: 7, 23: 0, 24: 17, 25: 0, 26: 4, 27: 3, 28: 6, 29: 1, 30: 3, 31: 0, 32: 37}</t>
         </is>
       </c>
     </row>
@@ -1248,6 +1343,17 @@
  [   0   92    0 ...    3    0   31]]</t>
         </is>
       </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>[[  0   1   0 ...   0   0   0]
+ [  0 441   0 ...   2   0   4]
+ [  0   0   0 ...   0   0   0]
+ ...
+ [  0   1   0 ...   0   0   0]
+ [  0   0   0 ...   0   0   0]
+ [  0   9   0 ...   0   0   1]]</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>